<commit_message>
Update the standard work files
</commit_message>
<xml_diff>
--- a/Hht.SampleInspection/Content/StandardWork/ValveSampleInspectionStandardWork.xlsx
+++ b/Hht.SampleInspection/Content/StandardWork/ValveSampleInspectionStandardWork.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukowiczj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukowiczj\Desktop\Sample Inspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="BK 879B LCR Meter 092915" sheetId="8" r:id="rId1"/>
-    <sheet name="Inductance Measurement Std Work" sheetId="9" r:id="rId2"/>
-    <sheet name=" Gas Valve Std Work 051116" sheetId="10" r:id="rId3"/>
+    <sheet name="Inductance Msmt Std Work 092916" sheetId="9" r:id="rId2"/>
+    <sheet name=" Gas Valve Std Work 061616" sheetId="10" r:id="rId3"/>
     <sheet name="3X Inspection Criteria" sheetId="13" r:id="rId4"/>
     <sheet name="Failure Modes 120815" sheetId="11" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
@@ -30,9 +30,9 @@
     <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">' Gas Valve Std Work 051116'!$A$1:$C$158</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">' Gas Valve Std Work 061616'!$A$1:$C$158</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'BK 879B LCR Meter 092915'!$A$1:$D$66</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Inductance Measurement Std Work'!$B$1:$C$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Inductance Msmt Std Work 092916'!$B$1:$C$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'SW - Valve Insp w Inductance '!$A$1:$H$105</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="336">
   <si>
     <t>Step</t>
   </si>
@@ -915,13 +915,7 @@
     <t>A Valve shall be rejected and sent to NCM if it does not meet the requirements of this Standard Work</t>
   </si>
   <si>
-    <t>If Valve is Dropped during the Sample Inspection Process, SCRAP VALVE, DO NOT COUNT AS FAIL, Document in Comment Section in Data Sheet.</t>
-  </si>
-  <si>
     <t>Turn on Pilot / Burner with Wall Switch or Remote Control.</t>
-  </si>
-  <si>
-    <t>Standard Work - Gas Valve Incoming Sample Inspection Process - DRAFT COPY</t>
   </si>
   <si>
     <r>
@@ -978,9 +972,6 @@
       </rPr>
       <t>Tab down</t>
     </r>
-  </si>
-  <si>
-    <t>/ ECM / Remote Control (if required)</t>
   </si>
   <si>
     <r>
@@ -1052,32 +1043,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> put a check mark on the label. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Remove Valve from test bench.  If the Valve passes, place black </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> mark just below the white identification label right above the circle cutout and replace in box.  If the Valve fails, click on "Edit This Part Received". This will take you back to the create screen. Click on "Individual Parts Comment" and write in a description of the failure. Tab down and fill in the NCM red tag number. Complete the NCM red tag and send the part to quality for confirmation testing.</t>
     </r>
   </si>
   <si>
@@ -1490,32 +1455,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Visually inspect Valve for missing / broken screws, debris in inlet / outlet ports/any damage </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Log results.                                                          </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tab down</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Measure "Pilot Valve Solenoid Inductance" by placing the red and black leads from the Multimeter on the valve (one of the leads will connect to the valve body and one of the leads will connect to the orange male connector on the valve). Flag if outside 250-650 mH.  </t>
     </r>
     <r>
@@ -1538,32 +1477,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>Tab down</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Measure "Main Valve Solenoid Inductance" by placing the red and black leads from the Multimeter on the valve (one of the leads will connect to the valve body and one of the leads will connect to the green male connector on the valve). Fflag if outside 350-700 mH. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Log results.                              </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Tab down.</t>
     </r>
   </si>
   <si>
@@ -1785,6 +1698,90 @@
   </si>
   <si>
     <t>Follow the NCM process for failed valves (reference the Failure Modes tab for lot / pallet rejection conditions).</t>
+  </si>
+  <si>
+    <t>If a Valve is DROPPED during the Sample Inspection Process, SCRAP VALVE, DO NOT COUNT AS FAIL, document as "DROPPED" in Individual Part Comments section of data entry screen.</t>
+  </si>
+  <si>
+    <t>Standard Work - Gas Valve Incoming Sample Inspection Process (ValveSampleInspectionStandardWork)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Visually inspect Valve for missing / broken screws, debris in inlet / outlet ports / any damage </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Log results.                                                          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tab down</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Measure "Main Valve Solenoid Inductance" by placing the red and black leads from the Multimeter on the valve (one of the leads will connect to the valve body and one of the leads will connect to the green male connector on the valve). Flag if outside 350-700 mH. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Log results.                              </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tab down.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remove Valve from test bench.  If the Valve passes, place black </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mark just below the white identification label right above the circle cutout and place back in box.  If the Valve fails, click on "Edit This Part Received". This will take you back to the create screen. Click on "Individual Parts Comment" and write in a description of the failure. Tab down and fill in the NCM red tag number. Complete the NCM red tag and send the part to quality for confirmation testing.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2574,7 +2571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2928,9 +2925,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3315,12 +3309,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="364102792"/>
-        <c:axId val="281959320"/>
+        <c:axId val="143165504"/>
+        <c:axId val="145144160"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="364102792"/>
+        <c:axId val="143165504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281959320"/>
+        <c:crossAx val="145144160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3355,7 +3349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="281959320"/>
+        <c:axId val="145144160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3383,7 +3377,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="364102792"/>
+        <c:crossAx val="143165504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3721,7 +3715,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="733425" y="9772651"/>
+          <a:off x="733425" y="9677401"/>
           <a:ext cx="6419850" cy="4029074"/>
           <a:chOff x="2617801" y="584276"/>
           <a:chExt cx="6858000" cy="5168728"/>
@@ -7273,7 +7267,7 @@
   <dimension ref="A1:AI106"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7296,7 +7290,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="52.5" x14ac:dyDescent="0.25">
@@ -7327,7 +7321,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="121" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -7729,46 +7723,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:3" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="153" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="154"/>
-      <c r="C2" s="155"/>
+    <row r="2" spans="1:3" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="152" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="153"/>
+      <c r="C2" s="154"/>
     </row>
     <row r="3" spans="1:3" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="167" t="s">
         <v>207</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="170"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="169"/>
     </row>
     <row r="4" spans="1:3" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="156"/>
-      <c r="B4" s="157"/>
-      <c r="C4" s="158"/>
+      <c r="A4" s="155"/>
+      <c r="B4" s="156"/>
+      <c r="C4" s="157"/>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="159" t="s">
-        <v>208</v>
-      </c>
-      <c r="B5" s="160"/>
-      <c r="C5" s="161"/>
+      <c r="A5" s="158" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="159"/>
+      <c r="C5" s="160"/>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="162"/>
-      <c r="B6" s="163"/>
-      <c r="C6" s="164"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="162"/>
-      <c r="B7" s="163"/>
-      <c r="C7" s="164"/>
+      <c r="A7" s="161"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="163"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="165"/>
-      <c r="B8" s="166"/>
-      <c r="C8" s="167"/>
+      <c r="A8" s="164"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
@@ -7786,7 +7780,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="108" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C10" s="94"/>
     </row>
@@ -7795,7 +7789,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="108" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C11" s="94"/>
     </row>
@@ -7804,7 +7798,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="108" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C12" s="94"/>
     </row>
@@ -7813,7 +7807,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="108" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C13" s="94"/>
     </row>
@@ -7822,7 +7816,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="108" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C14" s="94"/>
     </row>
@@ -7831,7 +7825,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="108" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C15" s="94"/>
     </row>
@@ -7840,168 +7834,165 @@
         <v>7</v>
       </c>
       <c r="B16" s="108" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C16" s="94"/>
     </row>
-    <row r="17" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="92">
         <v>8</v>
       </c>
       <c r="B17" s="108" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C17" s="94"/>
     </row>
-    <row r="18" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="92">
         <v>9</v>
       </c>
       <c r="B18" s="108" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C18" s="94"/>
     </row>
-    <row r="19" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="92">
         <v>10</v>
       </c>
       <c r="B19" s="108" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C19" s="94"/>
     </row>
-    <row r="20" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="126" x14ac:dyDescent="0.25">
       <c r="A20" s="36">
         <v>11</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C20" s="13"/>
     </row>
-    <row r="21" spans="1:6" ht="344.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="344.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36">
         <v>12</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C21" s="124"/>
     </row>
-    <row r="22" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="92">
         <v>13</v>
       </c>
       <c r="B22" s="108" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C22" s="94"/>
     </row>
-    <row r="23" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="A23" s="92">
         <v>14</v>
       </c>
       <c r="B23" s="108" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="92">
         <v>16</v>
       </c>
       <c r="B24" s="108" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="84" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="84" x14ac:dyDescent="0.25">
       <c r="A25" s="92">
         <v>17</v>
       </c>
       <c r="B25" s="108" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="F25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="92">
         <v>18</v>
       </c>
       <c r="B26" s="108" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" s="110">
         <v>19</v>
       </c>
       <c r="B27" s="111" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C27" s="125"/>
     </row>
-    <row r="28" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="110">
         <v>20</v>
       </c>
       <c r="B28" s="111" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C28" s="112"/>
     </row>
-    <row r="29" spans="1:6" ht="42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="42" x14ac:dyDescent="0.25">
       <c r="A29" s="116">
         <v>21</v>
       </c>
       <c r="B29" s="108" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C29" s="117" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="42" x14ac:dyDescent="0.25">
-      <c r="A30" s="126">
+    <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.25">
+      <c r="A30" s="116">
         <v>22</v>
       </c>
       <c r="B30" s="114" t="s">
-        <v>332</v>
-      </c>
-      <c r="C30" s="127" t="s">
+        <v>326</v>
+      </c>
+      <c r="C30" s="126" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="126" x14ac:dyDescent="0.25">
       <c r="A31" s="113">
         <v>23</v>
       </c>
       <c r="B31" s="114" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C31" s="115" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="126" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="126" x14ac:dyDescent="0.25">
       <c r="A32" s="92">
         <v>24</v>
       </c>
       <c r="B32" s="108" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C32" s="91" t="s">
         <v>166</v>
@@ -8012,7 +8003,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="108" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C33" s="117" t="s">
         <v>10</v>
@@ -8023,7 +8014,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="108" t="s">
-        <v>220</v>
+        <v>335</v>
       </c>
       <c r="C34" s="41"/>
     </row>
@@ -8032,7 +8023,7 @@
         <v>27</v>
       </c>
       <c r="B35" s="108" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C35" s="13"/>
     </row>
@@ -8041,7 +8032,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="108" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C36" s="13"/>
     </row>
@@ -8050,7 +8041,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="109" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C37" s="14"/>
     </row>
@@ -8917,73 +8908,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
-        <v>316</v>
-      </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
+      <c r="A1" s="127" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
-        <v>221</v>
-      </c>
-      <c r="B2" s="130" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
+      <c r="A2" s="128" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
       <c r="I2" s="47"/>
       <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="129"/>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
+      <c r="A3" s="128"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="129"/>
+      <c r="F3" s="129"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="129"/>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="129" t="s">
-        <v>223</v>
-      </c>
-      <c r="B4" s="130" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="130"/>
+      <c r="A4" s="128" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="129" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" s="129"/>
+      <c r="D4" s="129"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="129"/>
       <c r="I4" s="47"/>
       <c r="J4" s="47"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="129"/>
-      <c r="B6" s="131" t="s">
-        <v>225</v>
+      <c r="A6" s="128"/>
+      <c r="B6" s="130" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="132" t="s">
-        <v>226</v>
+      <c r="B7" s="131" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="132" t="s">
-        <v>227</v>
+      <c r="C8" s="131" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -8991,7 +8982,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -8999,7 +8990,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -9007,7 +8998,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -9015,98 +9006,98 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="129" t="s">
-        <v>232</v>
+      <c r="A13" s="128" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="133" t="s">
-        <v>233</v>
+      <c r="B14" s="132" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" s="132" t="s">
-        <v>234</v>
+      <c r="B15" s="131" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="132" t="s">
-        <v>235</v>
+      <c r="B16" s="131" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17" s="132" t="s">
-        <v>236</v>
+      <c r="B17" s="131" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="B18" s="132" t="s">
-        <v>237</v>
+      <c r="B18" s="131" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="133" t="s">
-        <v>238</v>
+      <c r="B20" s="132" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="130" t="s">
-        <v>239</v>
+      <c r="B21" s="129" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="130" t="s">
-        <v>240</v>
+      <c r="B22" s="129" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="133" t="s">
-        <v>241</v>
+      <c r="B24" s="132" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
-      <c r="B25" s="132" t="s">
-        <v>242</v>
+      <c r="B25" s="131" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="133" t="s">
-        <v>243</v>
+      <c r="B27" s="132" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" s="130" t="s">
-        <v>244</v>
+      <c r="B28" s="129" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="130" t="s">
-        <v>245</v>
+      <c r="B29" s="129" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -9114,113 +9105,113 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
-      <c r="B31" s="132" t="s">
-        <v>247</v>
+      <c r="B31" s="131" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="132" t="s">
-        <v>248</v>
+      <c r="B32" s="131" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
-      <c r="B33" s="132" t="s">
+      <c r="B33" s="131" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="133">
+        <v>4</v>
+      </c>
+      <c r="B34" s="131" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="133"/>
+      <c r="B35" s="131" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="133">
+        <v>5</v>
+      </c>
+      <c r="B36" s="131" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="133"/>
+      <c r="B37" s="131"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="130" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="134">
-        <v>4</v>
-      </c>
-      <c r="B34" s="132" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="130">
+        <v>1</v>
+      </c>
+      <c r="B39" s="130" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="134"/>
-      <c r="B35" s="132" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="131" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="134">
-        <v>5</v>
-      </c>
-      <c r="B36" s="132" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="130"/>
+      <c r="B41" s="134" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="134"/>
-      <c r="B37" s="132"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="131" t="s">
+      <c r="C41" s="135" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="131">
-        <v>1</v>
-      </c>
-      <c r="B39" s="131" t="s">
+      <c r="D41" s="135" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="132" t="s">
+      <c r="E41" s="136" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="131"/>
-      <c r="B41" s="135" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="130"/>
+      <c r="B42" s="137" t="s">
         <v>256</v>
       </c>
-      <c r="C41" s="136" t="s">
+      <c r="C42" s="135" t="s">
         <v>257</v>
       </c>
-      <c r="D41" s="136" t="s">
+      <c r="D42" s="138">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="138">
+        <v>0.05</v>
+      </c>
+      <c r="G42" s="131" t="s">
         <v>258</v>
       </c>
-      <c r="E41" s="137" t="s">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="130"/>
+      <c r="B43" s="139" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="131"/>
-      <c r="B42" s="138" t="s">
-        <v>260</v>
-      </c>
-      <c r="C42" s="136" t="s">
-        <v>261</v>
-      </c>
-      <c r="D42" s="139">
-        <v>0.5</v>
-      </c>
-      <c r="E42" s="139">
-        <v>0.05</v>
-      </c>
-      <c r="G42" s="132" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="131"/>
-      <c r="B43" s="140" t="s">
-        <v>263</v>
-      </c>
-      <c r="C43" s="136">
+      <c r="C43" s="135">
         <v>13</v>
       </c>
       <c r="D43" s="54">
@@ -9231,11 +9222,11 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="131"/>
-      <c r="B44" s="140" t="s">
-        <v>264</v>
-      </c>
-      <c r="C44" s="136">
+      <c r="A44" s="130"/>
+      <c r="B44" s="139" t="s">
+        <v>260</v>
+      </c>
+      <c r="C44" s="135">
         <v>20</v>
       </c>
       <c r="D44" s="54">
@@ -9247,16 +9238,16 @@
       <c r="G44">
         <v>1000</v>
       </c>
-      <c r="H44" s="132" t="s">
-        <v>265</v>
+      <c r="H44" s="131" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="131"/>
-      <c r="B45" s="140" t="s">
-        <v>266</v>
-      </c>
-      <c r="C45" s="136">
+      <c r="A45" s="130"/>
+      <c r="B45" s="139" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" s="135">
         <v>32</v>
       </c>
       <c r="D45" s="54">
@@ -9268,14 +9259,14 @@
       <c r="G45">
         <v>20</v>
       </c>
-      <c r="H45" s="132" t="s">
-        <v>267</v>
+      <c r="H45" s="131" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="131"/>
-      <c r="B46" s="140" t="s">
-        <v>268</v>
+      <c r="A46" s="130"/>
+      <c r="B46" s="139" t="s">
+        <v>264</v>
       </c>
       <c r="C46" s="54">
         <v>50</v>
@@ -9289,14 +9280,14 @@
       <c r="G46">
         <v>125</v>
       </c>
-      <c r="H46" s="137" t="s">
-        <v>269</v>
+      <c r="H46" s="136" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="131"/>
-      <c r="B47" s="140" t="s">
-        <v>270</v>
+      <c r="A47" s="130"/>
+      <c r="B47" s="139" t="s">
+        <v>266</v>
       </c>
       <c r="C47" s="54">
         <v>80</v>
@@ -9311,14 +9302,14 @@
         <f>G46/G45</f>
         <v>6.25</v>
       </c>
-      <c r="H47" s="132" t="s">
-        <v>271</v>
+      <c r="H47" s="131" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="131"/>
-      <c r="B48" s="140" t="s">
-        <v>272</v>
+      <c r="A48" s="130"/>
+      <c r="B48" s="139" t="s">
+        <v>268</v>
       </c>
       <c r="C48" s="54">
         <v>125</v>
@@ -9331,9 +9322,9 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="131"/>
-      <c r="B49" s="140" t="s">
-        <v>273</v>
+      <c r="A49" s="130"/>
+      <c r="B49" s="139" t="s">
+        <v>269</v>
       </c>
       <c r="C49" s="54">
         <v>200</v>
@@ -9346,9 +9337,9 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="131"/>
-      <c r="B50" s="140" t="s">
-        <v>274</v>
+      <c r="A50" s="130"/>
+      <c r="B50" s="139" t="s">
+        <v>270</v>
       </c>
       <c r="C50" s="54">
         <v>315</v>
@@ -9361,735 +9352,735 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="131"/>
-      <c r="B51" s="140"/>
+      <c r="A51" s="130"/>
+      <c r="B51" s="139"/>
       <c r="C51" s="54"/>
       <c r="D51" s="54"/>
       <c r="E51" s="54"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="141" t="s">
-        <v>275</v>
-      </c>
-      <c r="B52" s="137" t="s">
-        <v>276</v>
+      <c r="A52" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="B52" s="136" t="s">
+        <v>272</v>
       </c>
       <c r="C52" s="54"/>
       <c r="D52" s="54"/>
       <c r="E52" s="54"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="141"/>
-      <c r="B53" s="137" t="s">
-        <v>277</v>
+      <c r="A53" s="140"/>
+      <c r="B53" s="136" t="s">
+        <v>273</v>
       </c>
       <c r="C53" s="54"/>
       <c r="D53" s="54"/>
       <c r="E53" s="54"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="141" t="s">
+      <c r="A54" s="140" t="s">
+        <v>271</v>
+      </c>
+      <c r="B54" s="136" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="130"/>
+      <c r="B55" s="136" t="s">
         <v>275</v>
       </c>
-      <c r="B54" s="137" t="s">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="130"/>
+      <c r="B56" s="136"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="130">
+        <v>2</v>
+      </c>
+      <c r="B57" s="130" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="141" t="s">
+        <v>277</v>
+      </c>
+      <c r="B58" s="141" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="131"/>
-      <c r="B55" s="137" t="s">
+      <c r="C58" s="141" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="131"/>
-      <c r="B56" s="137"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="131">
-        <v>2</v>
-      </c>
-      <c r="B57" s="131" t="s">
+      <c r="D58" s="142" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="142" t="s">
+      <c r="E58" s="170" t="s">
         <v>281</v>
       </c>
-      <c r="B58" s="142" t="s">
+      <c r="F58" s="171"/>
+      <c r="G58" s="141"/>
+      <c r="H58" s="141"/>
+    </row>
+    <row r="59" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="141"/>
+      <c r="B59" s="141"/>
+      <c r="C59" s="141"/>
+      <c r="D59" s="141"/>
+      <c r="E59" s="141"/>
+      <c r="F59" s="141"/>
+      <c r="G59" s="141"/>
+      <c r="H59" s="141"/>
+    </row>
+    <row r="60" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="141"/>
+      <c r="B60" s="141"/>
+      <c r="C60" s="141" t="s">
         <v>282</v>
       </c>
-      <c r="C58" s="142" t="s">
+      <c r="D60" s="142" t="s">
         <v>283</v>
       </c>
-      <c r="D58" s="143" t="s">
+      <c r="E60" s="142" t="s">
         <v>284</v>
       </c>
-      <c r="E58" s="171" t="s">
+      <c r="F60" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G60" s="143" t="s">
         <v>285</v>
       </c>
-      <c r="F58" s="172"/>
-      <c r="G58" s="142"/>
-      <c r="H58" s="142"/>
-    </row>
-    <row r="59" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="142"/>
-      <c r="B59" s="142"/>
-      <c r="C59" s="142"/>
-      <c r="D59" s="142"/>
-      <c r="E59" s="142"/>
-      <c r="F59" s="142"/>
-      <c r="G59" s="142"/>
-      <c r="H59" s="142"/>
-    </row>
-    <row r="60" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="142"/>
-      <c r="B60" s="142"/>
-      <c r="C60" s="142" t="s">
+      <c r="H60" s="141"/>
+    </row>
+    <row r="61" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="141"/>
+      <c r="B61" s="141"/>
+      <c r="C61" s="141"/>
+      <c r="D61" s="141"/>
+      <c r="E61" s="142" t="s">
         <v>286</v>
       </c>
-      <c r="D60" s="143" t="s">
+      <c r="F61" s="142" t="s">
         <v>287</v>
       </c>
-      <c r="E60" s="143" t="s">
+      <c r="G61" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="H61" s="144" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="141"/>
+      <c r="B62" s="141"/>
+      <c r="C62" s="141"/>
+      <c r="D62" s="141"/>
+      <c r="E62" s="141"/>
+      <c r="F62" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="F60" s="143" t="s">
+      <c r="G62" s="142" t="s">
+        <v>285</v>
+      </c>
+      <c r="H62" s="145"/>
+    </row>
+    <row r="63" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="141"/>
+      <c r="B63" s="141"/>
+      <c r="C63" s="141"/>
+      <c r="D63" s="141"/>
+      <c r="E63" s="146" t="s">
+        <v>289</v>
+      </c>
+      <c r="F63" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="G63" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="H63" s="144" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="141"/>
+      <c r="B64" s="141"/>
+      <c r="C64" s="141"/>
+      <c r="D64" s="141"/>
+      <c r="E64" s="147"/>
+      <c r="F64" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="G64" s="142" t="s">
+        <v>285</v>
+      </c>
+      <c r="H64" s="145"/>
+    </row>
+    <row r="65" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="141"/>
+      <c r="B65" s="141"/>
+      <c r="C65" s="141"/>
+      <c r="D65" s="147"/>
+      <c r="E65" s="141"/>
+      <c r="F65" s="141"/>
+      <c r="G65" s="141"/>
+      <c r="H65" s="141"/>
+    </row>
+    <row r="66" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="141"/>
+      <c r="B66" s="141"/>
+      <c r="C66" s="141" t="s">
+        <v>290</v>
+      </c>
+      <c r="D66" s="142" t="s">
+        <v>283</v>
+      </c>
+      <c r="E66" s="142" t="s">
+        <v>284</v>
+      </c>
+      <c r="F66" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G66" s="143" t="s">
+        <v>285</v>
+      </c>
+      <c r="H66" s="141"/>
+    </row>
+    <row r="67" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="141"/>
+      <c r="B67" s="141"/>
+      <c r="C67" s="141"/>
+      <c r="D67" s="141"/>
+      <c r="E67" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="F67" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G67" s="143" t="s">
+        <v>285</v>
+      </c>
+      <c r="H67" s="141"/>
+    </row>
+    <row r="68" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="141"/>
+      <c r="B68" s="141"/>
+      <c r="C68" s="141"/>
+      <c r="D68" s="141"/>
+      <c r="E68" s="142" t="s">
+        <v>289</v>
+      </c>
+      <c r="F68" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G68" s="143" t="s">
+        <v>285</v>
+      </c>
+      <c r="H68" s="141"/>
+    </row>
+    <row r="69" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="141"/>
+      <c r="B69" s="141"/>
+      <c r="C69" s="141"/>
+      <c r="D69" s="141"/>
+      <c r="E69" s="141"/>
+      <c r="F69" s="141"/>
+      <c r="G69" s="141"/>
+      <c r="H69" s="141"/>
+    </row>
+    <row r="70" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="141" t="s">
+        <v>291</v>
+      </c>
+      <c r="B70" s="141" t="s">
+        <v>292</v>
+      </c>
+      <c r="C70" s="141" t="s">
+        <v>279</v>
+      </c>
+      <c r="D70" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="E70" s="170" t="s">
+        <v>293</v>
+      </c>
+      <c r="F70" s="171"/>
+      <c r="G70" s="141"/>
+      <c r="H70" s="141"/>
+    </row>
+    <row r="71" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="141"/>
+      <c r="B71" s="141"/>
+      <c r="C71" s="141"/>
+      <c r="D71" s="141"/>
+      <c r="E71" s="141"/>
+      <c r="F71" s="141"/>
+      <c r="G71" s="141"/>
+      <c r="H71" s="141"/>
+    </row>
+    <row r="72" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="141"/>
+      <c r="B72" s="141"/>
+      <c r="C72" s="141" t="s">
         <v>282</v>
       </c>
-      <c r="G60" s="144" t="s">
+      <c r="D72" s="142" t="s">
+        <v>283</v>
+      </c>
+      <c r="E72" s="142" t="s">
+        <v>284</v>
+      </c>
+      <c r="F72" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G72" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="H72" s="141"/>
+    </row>
+    <row r="73" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="141"/>
+      <c r="B73" s="141"/>
+      <c r="C73" s="141"/>
+      <c r="D73" s="141"/>
+      <c r="E73" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="F73" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="G73" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="H73" s="144" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="141"/>
+      <c r="B74" s="141"/>
+      <c r="C74" s="141"/>
+      <c r="D74" s="141"/>
+      <c r="E74" s="141"/>
+      <c r="F74" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="G74" s="142" t="s">
+        <v>294</v>
+      </c>
+      <c r="H74" s="145"/>
+    </row>
+    <row r="75" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="141"/>
+      <c r="B75" s="141"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="141"/>
+      <c r="E75" s="146" t="s">
         <v>289</v>
       </c>
-      <c r="H60" s="142"/>
-    </row>
-    <row r="61" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="142"/>
-      <c r="B61" s="142"/>
-      <c r="C61" s="142"/>
-      <c r="D61" s="142"/>
-      <c r="E61" s="143" t="s">
+      <c r="F75" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="G75" s="148" t="s">
+        <v>280</v>
+      </c>
+      <c r="H75" s="143" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="141"/>
+      <c r="B76" s="141"/>
+      <c r="C76" s="141"/>
+      <c r="D76" s="141"/>
+      <c r="E76" s="147"/>
+      <c r="F76" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="G76" s="142" t="s">
+        <v>295</v>
+      </c>
+      <c r="H76" s="145"/>
+    </row>
+    <row r="77" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="141"/>
+      <c r="B77" s="141"/>
+      <c r="C77" s="141"/>
+      <c r="D77" s="147"/>
+      <c r="E77" s="141"/>
+      <c r="F77" s="141"/>
+      <c r="G77" s="141"/>
+      <c r="H77" s="141"/>
+    </row>
+    <row r="78" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="141"/>
+      <c r="B78" s="141"/>
+      <c r="C78" s="141" t="s">
         <v>290</v>
       </c>
-      <c r="F61" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G61" s="143" t="s">
+      <c r="D78" s="142" t="s">
+        <v>283</v>
+      </c>
+      <c r="E78" s="142" t="s">
         <v>284</v>
       </c>
-      <c r="H61" s="145" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="142"/>
-      <c r="B62" s="142"/>
-      <c r="C62" s="142"/>
-      <c r="D62" s="142"/>
-      <c r="E62" s="142"/>
-      <c r="F62" s="143" t="s">
-        <v>292</v>
-      </c>
-      <c r="G62" s="143" t="s">
+      <c r="F78" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G78" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="H78" s="141"/>
+    </row>
+    <row r="79" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="141"/>
+      <c r="B79" s="141"/>
+      <c r="C79" s="141"/>
+      <c r="D79" s="141"/>
+      <c r="E79" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="F79" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G79" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="H79" s="141"/>
+    </row>
+    <row r="80" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="141"/>
+      <c r="B80" s="141"/>
+      <c r="C80" s="141"/>
+      <c r="D80" s="141"/>
+      <c r="E80" s="142" t="s">
         <v>289</v>
       </c>
-      <c r="H62" s="146"/>
-    </row>
-    <row r="63" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="142"/>
-      <c r="B63" s="142"/>
-      <c r="C63" s="142"/>
-      <c r="D63" s="142"/>
-      <c r="E63" s="147" t="s">
-        <v>293</v>
-      </c>
-      <c r="F63" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G63" s="143" t="s">
+      <c r="F80" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G80" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="H80" s="141"/>
+    </row>
+    <row r="81" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="141"/>
+      <c r="B81" s="141"/>
+      <c r="C81" s="141"/>
+      <c r="D81" s="141"/>
+      <c r="E81" s="141"/>
+      <c r="F81" s="141"/>
+      <c r="G81" s="141"/>
+      <c r="H81" s="141"/>
+    </row>
+    <row r="82" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="141" t="s">
+        <v>296</v>
+      </c>
+      <c r="B82" s="141" t="s">
+        <v>297</v>
+      </c>
+      <c r="C82" s="141" t="s">
+        <v>279</v>
+      </c>
+      <c r="D82" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="E82" s="172" t="s">
+        <v>298</v>
+      </c>
+      <c r="F82" s="173"/>
+      <c r="G82" s="141"/>
+      <c r="H82" s="141"/>
+    </row>
+    <row r="83" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="141"/>
+      <c r="B83" s="141"/>
+      <c r="C83" s="141"/>
+      <c r="D83" s="141"/>
+      <c r="E83" s="141"/>
+      <c r="F83" s="141"/>
+      <c r="G83" s="141"/>
+      <c r="H83" s="141"/>
+    </row>
+    <row r="84" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="141"/>
+      <c r="B84" s="141"/>
+      <c r="C84" s="141" t="s">
+        <v>282</v>
+      </c>
+      <c r="D84" s="142" t="s">
+        <v>283</v>
+      </c>
+      <c r="E84" s="142" t="s">
         <v>284</v>
       </c>
-      <c r="H63" s="145" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="142"/>
-      <c r="B64" s="142"/>
-      <c r="C64" s="142"/>
-      <c r="D64" s="142"/>
-      <c r="E64" s="148"/>
-      <c r="F64" s="143" t="s">
-        <v>292</v>
-      </c>
-      <c r="G64" s="143" t="s">
+      <c r="F84" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G84" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="H84" s="141"/>
+    </row>
+    <row r="85" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="141"/>
+      <c r="B85" s="141"/>
+      <c r="C85" s="141"/>
+      <c r="D85" s="141"/>
+      <c r="E85" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="F85" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="G85" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="H85" s="144" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="141"/>
+      <c r="B86" s="141"/>
+      <c r="C86" s="141"/>
+      <c r="D86" s="141"/>
+      <c r="E86" s="141"/>
+      <c r="F86" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="G86" s="142" t="s">
+        <v>294</v>
+      </c>
+      <c r="H86" s="145"/>
+    </row>
+    <row r="87" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="141"/>
+      <c r="B87" s="141"/>
+      <c r="C87" s="141"/>
+      <c r="D87" s="141"/>
+      <c r="E87" s="146" t="s">
         <v>289</v>
       </c>
-      <c r="H64" s="146"/>
-    </row>
-    <row r="65" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="142"/>
-      <c r="B65" s="142"/>
-      <c r="C65" s="142"/>
-      <c r="D65" s="148"/>
-      <c r="E65" s="142"/>
-      <c r="F65" s="142"/>
-      <c r="G65" s="142"/>
-      <c r="H65" s="142"/>
-    </row>
-    <row r="66" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="142"/>
-      <c r="B66" s="142"/>
-      <c r="C66" s="142" t="s">
+      <c r="F87" s="142" t="s">
+        <v>287</v>
+      </c>
+      <c r="G87" s="142" t="s">
+        <v>280</v>
+      </c>
+      <c r="H87" s="143" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="141"/>
+      <c r="B88" s="141"/>
+      <c r="C88" s="141"/>
+      <c r="D88" s="141"/>
+      <c r="E88" s="147"/>
+      <c r="F88" s="142" t="s">
+        <v>288</v>
+      </c>
+      <c r="G88" s="143" t="s">
+        <v>299</v>
+      </c>
+      <c r="H88" s="145"/>
+    </row>
+    <row r="89" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="141"/>
+      <c r="B89" s="141"/>
+      <c r="C89" s="141"/>
+      <c r="D89" s="147"/>
+      <c r="E89" s="141"/>
+      <c r="F89" s="141"/>
+      <c r="G89" s="141"/>
+      <c r="H89" s="141"/>
+    </row>
+    <row r="90" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="141"/>
+      <c r="B90" s="141"/>
+      <c r="C90" s="141" t="s">
+        <v>290</v>
+      </c>
+      <c r="D90" s="142" t="s">
+        <v>283</v>
+      </c>
+      <c r="E90" s="142" t="s">
+        <v>284</v>
+      </c>
+      <c r="F90" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G90" s="143" t="s">
         <v>294</v>
       </c>
-      <c r="D66" s="143" t="s">
-        <v>287</v>
-      </c>
-      <c r="E66" s="143" t="s">
-        <v>288</v>
-      </c>
-      <c r="F66" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G66" s="144" t="s">
+      <c r="H90" s="141"/>
+    </row>
+    <row r="91" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="141"/>
+      <c r="B91" s="141"/>
+      <c r="C91" s="141"/>
+      <c r="D91" s="141"/>
+      <c r="E91" s="142" t="s">
+        <v>286</v>
+      </c>
+      <c r="F91" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G91" s="143" t="s">
+        <v>294</v>
+      </c>
+      <c r="H91" s="141"/>
+    </row>
+    <row r="92" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="141"/>
+      <c r="B92" s="141"/>
+      <c r="C92" s="141"/>
+      <c r="D92" s="141"/>
+      <c r="E92" s="142" t="s">
         <v>289</v>
       </c>
-      <c r="H66" s="142"/>
-    </row>
-    <row r="67" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="142"/>
-      <c r="B67" s="142"/>
-      <c r="C67" s="142"/>
-      <c r="D67" s="142"/>
-      <c r="E67" s="143" t="s">
-        <v>290</v>
-      </c>
-      <c r="F67" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G67" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="H67" s="142"/>
-    </row>
-    <row r="68" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="142"/>
-      <c r="B68" s="142"/>
-      <c r="C68" s="142"/>
-      <c r="D68" s="142"/>
-      <c r="E68" s="143" t="s">
-        <v>293</v>
-      </c>
-      <c r="F68" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G68" s="144" t="s">
-        <v>289</v>
-      </c>
-      <c r="H68" s="142"/>
-    </row>
-    <row r="69" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="142"/>
-      <c r="B69" s="142"/>
-      <c r="C69" s="142"/>
-      <c r="D69" s="142"/>
-      <c r="E69" s="142"/>
-      <c r="F69" s="142"/>
-      <c r="G69" s="142"/>
-      <c r="H69" s="142"/>
-    </row>
-    <row r="70" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="142" t="s">
-        <v>295</v>
-      </c>
-      <c r="B70" s="142" t="s">
-        <v>296</v>
-      </c>
-      <c r="C70" s="142" t="s">
-        <v>283</v>
-      </c>
-      <c r="D70" s="143" t="s">
-        <v>284</v>
-      </c>
-      <c r="E70" s="171" t="s">
-        <v>297</v>
-      </c>
-      <c r="F70" s="172"/>
-      <c r="G70" s="142"/>
-      <c r="H70" s="142"/>
-    </row>
-    <row r="71" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="142"/>
-      <c r="B71" s="142"/>
-      <c r="C71" s="142"/>
-      <c r="D71" s="142"/>
-      <c r="E71" s="142"/>
-      <c r="F71" s="142"/>
-      <c r="G71" s="142"/>
-      <c r="H71" s="142"/>
-    </row>
-    <row r="72" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="142"/>
-      <c r="B72" s="142"/>
-      <c r="C72" s="142" t="s">
-        <v>286</v>
-      </c>
-      <c r="D72" s="143" t="s">
-        <v>287</v>
-      </c>
-      <c r="E72" s="143" t="s">
-        <v>288</v>
-      </c>
-      <c r="F72" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G72" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H72" s="142"/>
-    </row>
-    <row r="73" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="142"/>
-      <c r="B73" s="142"/>
-      <c r="C73" s="142"/>
-      <c r="D73" s="142"/>
-      <c r="E73" s="143" t="s">
-        <v>290</v>
-      </c>
-      <c r="F73" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G73" s="143" t="s">
-        <v>284</v>
-      </c>
-      <c r="H73" s="145" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="142"/>
-      <c r="B74" s="142"/>
-      <c r="C74" s="142"/>
-      <c r="D74" s="142"/>
-      <c r="E74" s="142"/>
-      <c r="F74" s="143" t="s">
-        <v>292</v>
-      </c>
-      <c r="G74" s="143" t="s">
-        <v>298</v>
-      </c>
-      <c r="H74" s="146"/>
-    </row>
-    <row r="75" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="142"/>
-      <c r="B75" s="142"/>
-      <c r="C75" s="142"/>
-      <c r="D75" s="142"/>
-      <c r="E75" s="147" t="s">
-        <v>293</v>
-      </c>
-      <c r="F75" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G75" s="149" t="s">
-        <v>284</v>
-      </c>
-      <c r="H75" s="144" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="142"/>
-      <c r="B76" s="142"/>
-      <c r="C76" s="142"/>
-      <c r="D76" s="142"/>
-      <c r="E76" s="148"/>
-      <c r="F76" s="143" t="s">
-        <v>292</v>
-      </c>
-      <c r="G76" s="143" t="s">
-        <v>299</v>
-      </c>
-      <c r="H76" s="146"/>
-    </row>
-    <row r="77" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="142"/>
-      <c r="B77" s="142"/>
-      <c r="C77" s="142"/>
-      <c r="D77" s="148"/>
-      <c r="E77" s="142"/>
-      <c r="F77" s="142"/>
-      <c r="G77" s="142"/>
-      <c r="H77" s="142"/>
-    </row>
-    <row r="78" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="142"/>
-      <c r="B78" s="142"/>
-      <c r="C78" s="142" t="s">
+      <c r="F92" s="142" t="s">
+        <v>278</v>
+      </c>
+      <c r="G92" s="143" t="s">
         <v>294</v>
       </c>
-      <c r="D78" s="143" t="s">
-        <v>287</v>
-      </c>
-      <c r="E78" s="143" t="s">
-        <v>288</v>
-      </c>
-      <c r="F78" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G78" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H78" s="142"/>
-    </row>
-    <row r="79" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="142"/>
-      <c r="B79" s="142"/>
-      <c r="C79" s="142"/>
-      <c r="D79" s="142"/>
-      <c r="E79" s="143" t="s">
-        <v>290</v>
-      </c>
-      <c r="F79" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G79" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H79" s="142"/>
-    </row>
-    <row r="80" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="142"/>
-      <c r="B80" s="142"/>
-      <c r="C80" s="142"/>
-      <c r="D80" s="142"/>
-      <c r="E80" s="143" t="s">
-        <v>293</v>
-      </c>
-      <c r="F80" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G80" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H80" s="142"/>
-    </row>
-    <row r="81" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="142"/>
-      <c r="B81" s="142"/>
-      <c r="C81" s="142"/>
-      <c r="D81" s="142"/>
-      <c r="E81" s="142"/>
-      <c r="F81" s="142"/>
-      <c r="G81" s="142"/>
-      <c r="H81" s="142"/>
-    </row>
-    <row r="82" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="142" t="s">
-        <v>300</v>
-      </c>
-      <c r="B82" s="142" t="s">
-        <v>301</v>
-      </c>
-      <c r="C82" s="142" t="s">
-        <v>283</v>
-      </c>
-      <c r="D82" s="143" t="s">
-        <v>284</v>
-      </c>
-      <c r="E82" s="173" t="s">
-        <v>302</v>
-      </c>
-      <c r="F82" s="174"/>
-      <c r="G82" s="142"/>
-      <c r="H82" s="142"/>
-    </row>
-    <row r="83" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="142"/>
-      <c r="B83" s="142"/>
-      <c r="C83" s="142"/>
-      <c r="D83" s="142"/>
-      <c r="E83" s="142"/>
-      <c r="F83" s="142"/>
-      <c r="G83" s="142"/>
-      <c r="H83" s="142"/>
-    </row>
-    <row r="84" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="142"/>
-      <c r="B84" s="142"/>
-      <c r="C84" s="142" t="s">
-        <v>286</v>
-      </c>
-      <c r="D84" s="143" t="s">
-        <v>287</v>
-      </c>
-      <c r="E84" s="143" t="s">
-        <v>288</v>
-      </c>
-      <c r="F84" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G84" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H84" s="142"/>
-    </row>
-    <row r="85" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="142"/>
-      <c r="B85" s="142"/>
-      <c r="C85" s="142"/>
-      <c r="D85" s="142"/>
-      <c r="E85" s="143" t="s">
-        <v>290</v>
-      </c>
-      <c r="F85" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G85" s="143" t="s">
-        <v>284</v>
-      </c>
-      <c r="H85" s="145" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="142"/>
-      <c r="B86" s="142"/>
-      <c r="C86" s="142"/>
-      <c r="D86" s="142"/>
-      <c r="E86" s="142"/>
-      <c r="F86" s="143" t="s">
-        <v>292</v>
-      </c>
-      <c r="G86" s="143" t="s">
-        <v>298</v>
-      </c>
-      <c r="H86" s="146"/>
-    </row>
-    <row r="87" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="142"/>
-      <c r="B87" s="142"/>
-      <c r="C87" s="142"/>
-      <c r="D87" s="142"/>
-      <c r="E87" s="147" t="s">
-        <v>293</v>
-      </c>
-      <c r="F87" s="143" t="s">
-        <v>291</v>
-      </c>
-      <c r="G87" s="143" t="s">
-        <v>284</v>
-      </c>
-      <c r="H87" s="144" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="142"/>
-      <c r="B88" s="142"/>
-      <c r="C88" s="142"/>
-      <c r="D88" s="142"/>
-      <c r="E88" s="148"/>
-      <c r="F88" s="143" t="s">
-        <v>292</v>
-      </c>
-      <c r="G88" s="144" t="s">
-        <v>303</v>
-      </c>
-      <c r="H88" s="146"/>
-    </row>
-    <row r="89" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="142"/>
-      <c r="B89" s="142"/>
-      <c r="C89" s="142"/>
-      <c r="D89" s="148"/>
-      <c r="E89" s="142"/>
-      <c r="F89" s="142"/>
-      <c r="G89" s="142"/>
-      <c r="H89" s="142"/>
-    </row>
-    <row r="90" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="142"/>
-      <c r="B90" s="142"/>
-      <c r="C90" s="142" t="s">
-        <v>294</v>
-      </c>
-      <c r="D90" s="143" t="s">
-        <v>287</v>
-      </c>
-      <c r="E90" s="143" t="s">
-        <v>288</v>
-      </c>
-      <c r="F90" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G90" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H90" s="142"/>
-    </row>
-    <row r="91" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="142"/>
-      <c r="B91" s="142"/>
-      <c r="C91" s="142"/>
-      <c r="D91" s="142"/>
-      <c r="E91" s="143" t="s">
-        <v>290</v>
-      </c>
-      <c r="F91" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G91" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H91" s="142"/>
-    </row>
-    <row r="92" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="142"/>
-      <c r="B92" s="142"/>
-      <c r="C92" s="142"/>
-      <c r="D92" s="142"/>
-      <c r="E92" s="143" t="s">
-        <v>293</v>
-      </c>
-      <c r="F92" s="143" t="s">
-        <v>282</v>
-      </c>
-      <c r="G92" s="144" t="s">
-        <v>298</v>
-      </c>
-      <c r="H92" s="142"/>
+      <c r="H92" s="141"/>
     </row>
     <row r="93" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="94" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="148" t="s">
-        <v>304</v>
-      </c>
-      <c r="B94" s="148" t="s">
-        <v>305</v>
-      </c>
-      <c r="C94" s="150"/>
-      <c r="D94" s="150"/>
-      <c r="E94" s="150"/>
-      <c r="F94" s="150"/>
-      <c r="G94" s="150"/>
-      <c r="H94" s="150"/>
+      <c r="A94" s="147" t="s">
+        <v>300</v>
+      </c>
+      <c r="B94" s="147" t="s">
+        <v>301</v>
+      </c>
+      <c r="C94" s="149"/>
+      <c r="D94" s="149"/>
+      <c r="E94" s="149"/>
+      <c r="F94" s="149"/>
+      <c r="G94" s="149"/>
+      <c r="H94" s="149"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="131">
+      <c r="A96" s="130">
         <v>3</v>
       </c>
-      <c r="B96" s="131" t="s">
-        <v>306</v>
+      <c r="B96" s="130" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>1</v>
       </c>
-      <c r="C97" s="132" t="s">
+      <c r="C97" s="131" t="s">
+        <v>303</v>
+      </c>
+      <c r="D97" s="131"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="131"/>
+      <c r="C98" s="131" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="131"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="131">
+        <v>2</v>
+      </c>
+      <c r="C99" s="131" t="s">
+        <v>305</v>
+      </c>
+      <c r="D99" s="131"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="131" t="s">
+        <v>306</v>
+      </c>
+      <c r="D100" s="131"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="150"/>
+      <c r="C101" s="131" t="s">
         <v>307</v>
       </c>
-      <c r="D97" s="132"/>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="132"/>
-      <c r="C98" s="132" t="s">
+      <c r="D101" s="131"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="131">
+        <v>3</v>
+      </c>
+      <c r="C102" s="131" t="s">
         <v>308</v>
       </c>
-      <c r="D98" s="132"/>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="132">
-        <v>2</v>
-      </c>
-      <c r="C99" s="132" t="s">
+      <c r="D102" s="131"/>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="131"/>
+      <c r="C103" s="131" t="s">
         <v>309</v>
       </c>
-      <c r="D99" s="132"/>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C100" s="132" t="s">
+      <c r="D103" s="131"/>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="131" t="s">
         <v>310</v>
       </c>
-      <c r="D100" s="132"/>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="151"/>
-      <c r="C101" s="132" t="s">
+      <c r="D104" s="131"/>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="131">
+        <v>4</v>
+      </c>
+      <c r="C105" s="131" t="s">
         <v>311</v>
       </c>
-      <c r="D101" s="132"/>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="132">
-        <v>3</v>
-      </c>
-      <c r="C102" s="132" t="s">
-        <v>312</v>
-      </c>
-      <c r="D102" s="132"/>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="132"/>
-      <c r="C103" s="132" t="s">
-        <v>313</v>
-      </c>
-      <c r="D103" s="132"/>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C104" s="132" t="s">
-        <v>314</v>
-      </c>
-      <c r="D104" s="132"/>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="132">
-        <v>4</v>
-      </c>
-      <c r="C105" s="132" t="s">
-        <v>315</v>
-      </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="152"/>
+      <c r="B106" s="151"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="152"/>
+      <c r="B107" s="151"/>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="152"/>
+      <c r="B108" s="151"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="152"/>
+      <c r="B109" s="151"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="152"/>
+      <c r="B110" s="151"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="152"/>
+      <c r="B111" s="151"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="132"/>
+      <c r="B112" s="131"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="132"/>
+      <c r="B113" s="131"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="132"/>
+      <c r="B114" s="131"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="132"/>
+      <c r="B115" s="131"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="132"/>
+      <c r="B116" s="131"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="132"/>
+      <c r="B117" s="131"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="132"/>
+      <c r="B118" s="131"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10343,7 +10334,7 @@
       <c r="B27" s="106" t="s">
         <v>200</v>
       </c>
-      <c r="C27" s="175" t="s">
+      <c r="C27" s="174" t="s">
         <v>201</v>
       </c>
     </row>
@@ -10352,21 +10343,21 @@
       <c r="B28" s="106" t="s">
         <v>202</v>
       </c>
-      <c r="C28" s="175"/>
+      <c r="C28" s="174"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="106" t="s">
         <v>203</v>
       </c>
-      <c r="C29" s="175"/>
+      <c r="C29" s="174"/>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="106" t="s">
         <v>204</v>
       </c>
-      <c r="C30" s="175"/>
+      <c r="C30" s="174"/>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="25">
@@ -10452,11 +10443,11 @@
     <row r="1" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:39" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="176" t="s">
+      <c r="B2" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="177"/>
-      <c r="D2" s="178"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="46"/>
       <c r="F2" s="73" t="s">
         <v>0</v>
@@ -10466,11 +10457,11 @@
       </c>
     </row>
     <row r="3" spans="1:39" ht="53.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="156" t="s">
+      <c r="B3" s="155" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="157"/>
       <c r="E3" s="45"/>
       <c r="F3" s="57">
         <v>1</v>
@@ -10903,26 +10894,26 @@
       <c r="D23" s="15"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="159" t="s">
+      <c r="B24" s="158" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="160"/>
-      <c r="D24" s="161"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="160"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="162"/>
-      <c r="C25" s="163"/>
-      <c r="D25" s="164"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="162"/>
+      <c r="D25" s="163"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="162"/>
-      <c r="C26" s="163"/>
-      <c r="D26" s="164"/>
+      <c r="B26" s="161"/>
+      <c r="C26" s="162"/>
+      <c r="D26" s="163"/>
     </row>
     <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="165"/>
-      <c r="C27" s="166"/>
-      <c r="D27" s="167"/>
+      <c r="B27" s="164"/>
+      <c r="C27" s="165"/>
+      <c r="D27" s="166"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
@@ -11051,127 +11042,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="184" t="s">
+      <c r="A1" s="183" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="186"/>
+      <c r="B1" s="184"/>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="185"/>
     </row>
     <row r="2" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="187" t="s">
+      <c r="A2" s="186" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="188"/>
-      <c r="C2" s="189" t="s">
+      <c r="B2" s="187"/>
+      <c r="C2" s="188" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="190"/>
+      <c r="D2" s="189"/>
       <c r="E2" s="51" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="191" t="s">
+      <c r="A3" s="190" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="189" t="s">
+      <c r="B3" s="191"/>
+      <c r="C3" s="188" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="192"/>
+      <c r="D3" s="191"/>
       <c r="E3" s="52" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="181" t="s">
+      <c r="A4" s="180" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="182"/>
-      <c r="C4" s="182" t="s">
+      <c r="B4" s="181"/>
+      <c r="C4" s="181" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="182"/>
+      <c r="D4" s="181"/>
       <c r="E4" s="50" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="179" t="s">
+      <c r="A5" s="178" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="180"/>
-      <c r="C5" s="180" t="s">
+      <c r="B5" s="179"/>
+      <c r="C5" s="179" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="180"/>
+      <c r="D5" s="179"/>
       <c r="E5" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="179" t="s">
+      <c r="A6" s="178" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="180"/>
-      <c r="C6" s="180" t="s">
+      <c r="B6" s="179"/>
+      <c r="C6" s="179" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="180"/>
+      <c r="D6" s="179"/>
       <c r="E6" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="179" t="s">
+      <c r="A7" s="178" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="180"/>
-      <c r="C7" s="180" t="s">
+      <c r="B7" s="179"/>
+      <c r="C7" s="179" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="180"/>
+      <c r="D7" s="179"/>
       <c r="E7" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="179" t="s">
+      <c r="A8" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="180"/>
-      <c r="C8" s="180" t="s">
+      <c r="B8" s="179"/>
+      <c r="C8" s="179" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="180"/>
+      <c r="D8" s="179"/>
       <c r="E8" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="179" t="s">
+      <c r="A9" s="178" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="180"/>
-      <c r="C9" s="180" t="s">
+      <c r="B9" s="179"/>
+      <c r="C9" s="179" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="180"/>
+      <c r="D9" s="179"/>
       <c r="E9" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="49" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="181" t="s">
+      <c r="A10" s="180" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="182"/>
-      <c r="C10" s="183" t="s">
+      <c r="B10" s="181"/>
+      <c r="C10" s="182" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="179"/>
+      <c r="D10" s="178"/>
       <c r="E10" s="48" t="s">
         <v>106</v>
       </c>
@@ -40872,75 +40863,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="192" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="195"/>
+      <c r="B1" s="193"/>
+      <c r="C1" s="193"/>
+      <c r="D1" s="193"/>
+      <c r="E1" s="194"/>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="195" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="197"/>
-      <c r="C2" s="198" t="s">
+      <c r="B2" s="196"/>
+      <c r="C2" s="197" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="199"/>
+      <c r="D2" s="198"/>
       <c r="E2" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="199" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="201"/>
-      <c r="C3" s="198" t="s">
+      <c r="B3" s="200"/>
+      <c r="C3" s="197" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="201"/>
+      <c r="D3" s="200"/>
       <c r="E3" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="201" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="203"/>
-      <c r="C4" s="203" t="s">
+      <c r="B4" s="202"/>
+      <c r="C4" s="202" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="203"/>
+      <c r="D4" s="202"/>
       <c r="E4" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="202" t="s">
+      <c r="A5" s="201" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="203"/>
-      <c r="C5" s="203" t="s">
+      <c r="B5" s="202"/>
+      <c r="C5" s="202" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="203"/>
+      <c r="D5" s="202"/>
       <c r="E5" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="202" t="s">
+      <c r="A6" s="201" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="203"/>
-      <c r="C6" s="203" t="s">
+      <c r="B6" s="202"/>
+      <c r="C6" s="202" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="203"/>
+      <c r="D6" s="202"/>
       <c r="E6" s="53" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
Moved Serial number position in the screen (to be above Incoming Date) to avoid issues with scanner
</commit_message>
<xml_diff>
--- a/Hht.SampleInspection/Content/StandardWork/ValveSampleInspectionStandardWork.xlsx
+++ b/Hht.SampleInspection/Content/StandardWork/ValveSampleInspectionStandardWork.xlsx
@@ -3053,19 +3053,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3094,6 +3091,17 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3129,14 +3137,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -3309,12 +3309,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="cylinder"/>
-        <c:axId val="143165504"/>
-        <c:axId val="145144160"/>
+        <c:axId val="170400640"/>
+        <c:axId val="171914816"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="143165504"/>
+        <c:axId val="170400640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3341,7 +3341,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145144160"/>
+        <c:crossAx val="171914816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3349,7 +3349,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145144160"/>
+        <c:axId val="171914816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3377,7 +3377,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143165504"/>
+        <c:crossAx val="170400640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11042,127 +11042,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="183" t="s">
+      <c r="A1" s="182" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="184"/>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="185"/>
+      <c r="B1" s="183"/>
+      <c r="C1" s="183"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="184"/>
     </row>
     <row r="2" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="187"/>
-      <c r="C2" s="188" t="s">
+      <c r="B2" s="186"/>
+      <c r="C2" s="187" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="189"/>
+      <c r="D2" s="188"/>
       <c r="E2" s="51" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="190" t="s">
+      <c r="A3" s="189" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="191"/>
-      <c r="C3" s="188" t="s">
+      <c r="B3" s="190"/>
+      <c r="C3" s="187" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="191"/>
+      <c r="D3" s="190"/>
       <c r="E3" s="52" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="180" t="s">
+      <c r="A4" s="178" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="181"/>
-      <c r="C4" s="181" t="s">
+      <c r="B4" s="179"/>
+      <c r="C4" s="179" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="181"/>
+      <c r="D4" s="179"/>
       <c r="E4" s="50" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="178" t="s">
+      <c r="A5" s="180" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="179"/>
-      <c r="C5" s="179" t="s">
+      <c r="B5" s="181"/>
+      <c r="C5" s="181" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="179"/>
+      <c r="D5" s="181"/>
       <c r="E5" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="178" t="s">
+      <c r="A6" s="180" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="179"/>
-      <c r="C6" s="179" t="s">
+      <c r="B6" s="181"/>
+      <c r="C6" s="181" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="179"/>
+      <c r="D6" s="181"/>
       <c r="E6" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="178" t="s">
+      <c r="A7" s="180" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="179"/>
-      <c r="C7" s="179" t="s">
+      <c r="B7" s="181"/>
+      <c r="C7" s="181" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="179"/>
+      <c r="D7" s="181"/>
       <c r="E7" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="178" t="s">
+      <c r="A8" s="180" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="179"/>
-      <c r="C8" s="179" t="s">
+      <c r="B8" s="181"/>
+      <c r="C8" s="181" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="179"/>
+      <c r="D8" s="181"/>
       <c r="E8" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="49" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="178" t="s">
+      <c r="A9" s="180" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="179"/>
-      <c r="C9" s="179" t="s">
+      <c r="B9" s="181"/>
+      <c r="C9" s="181" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="179"/>
+      <c r="D9" s="181"/>
       <c r="E9" s="48" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="49" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="180" t="s">
+      <c r="A10" s="178" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="181"/>
-      <c r="C10" s="182" t="s">
+      <c r="B10" s="179"/>
+      <c r="C10" s="191" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="178"/>
+      <c r="D10" s="180"/>
       <c r="E10" s="48" t="s">
         <v>106</v>
       </c>
@@ -40822,15 +40822,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A10:B10"/>
@@ -40841,6 +40832,15 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -40863,92 +40863,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="192" t="s">
+      <c r="A1" s="194" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="194"/>
+      <c r="B1" s="195"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="195"/>
+      <c r="E1" s="196"/>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="195" t="s">
+      <c r="A2" s="197" t="s">
         <v>125</v>
       </c>
-      <c r="B2" s="196"/>
-      <c r="C2" s="197" t="s">
+      <c r="B2" s="198"/>
+      <c r="C2" s="199" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="198"/>
+      <c r="D2" s="200"/>
       <c r="E2" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="199" t="s">
+      <c r="A3" s="201" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="200"/>
-      <c r="C3" s="197" t="s">
+      <c r="B3" s="202"/>
+      <c r="C3" s="199" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="200"/>
+      <c r="D3" s="202"/>
       <c r="E3" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="192" t="s">
         <v>128</v>
       </c>
-      <c r="B4" s="202"/>
-      <c r="C4" s="202" t="s">
+      <c r="B4" s="193"/>
+      <c r="C4" s="193" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="202"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="192" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="202"/>
-      <c r="C5" s="202" t="s">
+      <c r="B5" s="193"/>
+      <c r="C5" s="193" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="202"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="53" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="201" t="s">
+      <c r="A6" s="192" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="202"/>
-      <c r="C6" s="202" t="s">
+      <c r="B6" s="193"/>
+      <c r="C6" s="193" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="202"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="53" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>